<commit_message>
24 SCHOOLS LIST HAS BEEN UPDATED
24 SCHOOLS LIST HAS BEEN UPDATED
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools - Rahul.xlsx
+++ b/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools - Rahul.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Marketing\AI marketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83E40AF-091C-4A39-8792-5FDCE75EB9D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A38408-5454-4C53-BCEE-59FDA3621974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
   <si>
     <t>Slno</t>
   </si>
@@ -107,13 +107,145 @@
   </si>
   <si>
     <t>Email ID</t>
+  </si>
+  <si>
+    <t>Calcutta Boys (Main)</t>
+  </si>
+  <si>
+    <t>I.C.S.E</t>
+  </si>
+  <si>
+    <t>cbsmain@calcuttaboysschools.org</t>
+  </si>
+  <si>
+    <t>JJ. Ajmera</t>
+  </si>
+  <si>
+    <t>BGES</t>
+  </si>
+  <si>
+    <t>bges12@gmail.com</t>
+  </si>
+  <si>
+    <t>Khalsa</t>
+  </si>
+  <si>
+    <t>WB</t>
+  </si>
+  <si>
+    <t>@khs_kol@yahoo.in</t>
+  </si>
+  <si>
+    <t>De Paul (Bansdroni)</t>
+  </si>
+  <si>
+    <t>depaulbansdroni@gmail.com</t>
+  </si>
+  <si>
+    <t>De Paul( Jaynpur)</t>
+  </si>
+  <si>
+    <t>National Public School</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silver Point </t>
+  </si>
+  <si>
+    <t>CBSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Garden High </t>
+  </si>
+  <si>
+    <t>principal@gardenhighschool.org</t>
+  </si>
+  <si>
+    <t>DPS NEWTOWN</t>
+  </si>
+  <si>
+    <t>admin@dpsn.org.in</t>
+  </si>
+  <si>
+    <t>DPS MEGACITY</t>
+  </si>
+  <si>
+    <t>enquiry@dpsmegacity.in</t>
+  </si>
+  <si>
+    <t>South End</t>
+  </si>
+  <si>
+    <t>Better High</t>
+  </si>
+  <si>
+    <t>Miranda</t>
+  </si>
+  <si>
+    <t>Dolna Day</t>
+  </si>
+  <si>
+    <t>03324424102\07980451826</t>
+  </si>
+  <si>
+    <t>K.E Carmel Amtala</t>
+  </si>
+  <si>
+    <t>dolnaday@gmail.com</t>
+  </si>
+  <si>
+    <t>kecarmel@gmail.com</t>
+  </si>
+  <si>
+    <t>Central Model School Amatala</t>
+  </si>
+  <si>
+    <t>amtalacms@gmail.com</t>
+  </si>
+  <si>
+    <t>Matrix Model School</t>
+  </si>
+  <si>
+    <t>mmschool212yahoo.co.in</t>
+  </si>
+  <si>
+    <t>Jyotirmoy School</t>
+  </si>
+  <si>
+    <t>principal@jpsedu.in</t>
+  </si>
+  <si>
+    <t>Don Bosco</t>
+  </si>
+  <si>
+    <t>dbkolkata@gmail.com</t>
+  </si>
+  <si>
+    <t>St.James</t>
+  </si>
+  <si>
+    <t>sjskolkata@gmail.com</t>
+  </si>
+  <si>
+    <t>Pratt Memorial</t>
+  </si>
+  <si>
+    <t>prattmemorialschool@yahoo.com</t>
+  </si>
+  <si>
+    <t>Jewish Girls</t>
+  </si>
+  <si>
+    <t>jewishgirls1881@gmail.com</t>
+  </si>
+  <si>
+    <t>St.Thomas Boys</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,12 +301,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF422E59"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -197,7 +323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -218,7 +344,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -503,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,48 +698,420 @@
         <v>14</v>
       </c>
     </row>
+    <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1">
+        <v>3322651531</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3324753015</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3340196666</v>
+      </c>
+    </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3324753765</v>
+      </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="E7" s="7"/>
+    <row r="6" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3324286903</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="7">
+        <v>8902488077</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="E8" s="8"/>
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="8">
+        <v>9163741069</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="E9" s="8"/>
-    </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D22" s="10"/>
-    </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D23" s="6"/>
-    </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="8">
+        <v>3324411691</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3324413804</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="1">
+        <v>9830688888</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="1">
+        <v>9073985531</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3324712220</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="1">
+        <v>3324131158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="1">
+        <v>9836242629</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="1">
+        <v>9051973905</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="1">
+        <v>9674850783</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="1">
+        <v>9674111783</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="1">
+        <v>33218260082</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="1">
+        <v>3322879202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="1">
+        <v>3322841546</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="1">
+        <v>3322484593</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="1">
+        <v>3322297741</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="D25" s="9"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D26" s="11"/>
-    </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D27" s="11"/>
-    </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D28" s="11"/>
-    </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D26" s="10"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D27" s="10"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D28" s="10"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D32" s="6"/>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D33" s="6"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{7E50E3B3-C867-48D0-9918-D378D6E08E45}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{F62EC26A-C33A-4D48-B85C-D3EB3A8908C3}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{5C4E76F8-B0C8-4530-BE63-DA12B23A6D11}"/>
+    <hyperlink ref="D10" r:id="rId4" xr:uid="{064D48A3-BF4B-40BC-AEDF-B1FDB3331A79}"/>
+    <hyperlink ref="D11" r:id="rId5" xr:uid="{ACF742C5-CA10-4D05-97D5-0430A9817149}"/>
+    <hyperlink ref="D12" r:id="rId6" xr:uid="{63F22DFA-3CD8-4976-AF91-EEA0C9361DF2}"/>
+    <hyperlink ref="D16" r:id="rId7" xr:uid="{BFAB8F28-BD55-4BF7-9BA4-58D779CAD47D}"/>
+    <hyperlink ref="D17" r:id="rId8" xr:uid="{D28C1110-1971-42A0-B310-E52E34FB8FFD}"/>
+    <hyperlink ref="D18" r:id="rId9" xr:uid="{61902B7B-79C2-4173-B57D-8EA4A58B9DD2}"/>
+    <hyperlink ref="D20" r:id="rId10" xr:uid="{A65AC219-C996-4CB2-8138-5CA673E45FA3}"/>
+    <hyperlink ref="D21" r:id="rId11" xr:uid="{AF7AEA0F-6E74-4724-9610-0E480B5D432F}"/>
+    <hyperlink ref="D22" r:id="rId12" xr:uid="{07F0AFEA-F8BD-4093-81BD-41EC84D474F1}"/>
+    <hyperlink ref="D23" r:id="rId13" xr:uid="{C476D3FD-7619-4152-BF8B-DA12B03063BD}"/>
+    <hyperlink ref="D24" r:id="rId14" xr:uid="{380E3A26-AE6E-419B-A807-E6BB4359E95A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
+  <legacyDrawing r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
41 more schools updated
41 more schools updated
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools - Rahul.xlsx
+++ b/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools - Rahul.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Marketing\AI marketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A38408-5454-4C53-BCEE-59FDA3621974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B17D572-0F56-4228-A5AC-7464C6D374E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="129">
   <si>
     <t>Slno</t>
   </si>
@@ -238,14 +238,221 @@
     <t>jewishgirls1881@gmail.com</t>
   </si>
   <si>
-    <t>St.Thomas Boys</t>
+    <t>St.Thomas Boys( Kidderpore)</t>
+  </si>
+  <si>
+    <t>principal@stsboys.com</t>
+  </si>
+  <si>
+    <t>St.Helen</t>
+  </si>
+  <si>
+    <t>st.helen@yahoo.co.in</t>
+  </si>
+  <si>
+    <t>Hartley</t>
+  </si>
+  <si>
+    <t>saratboseroad@hartley.co.in</t>
+  </si>
+  <si>
+    <t>Indian Public School( Howrah)</t>
+  </si>
+  <si>
+    <t>enquiries@ipshowrah.com</t>
+  </si>
+  <si>
+    <t>07044304551\52</t>
+  </si>
+  <si>
+    <t>Sri Sri Academy</t>
+  </si>
+  <si>
+    <t>barry.antunis@ssa.org.in</t>
+  </si>
+  <si>
+    <t>Gokhale Memorial</t>
+  </si>
+  <si>
+    <t>gokhale_memorial@yahoo.com</t>
+  </si>
+  <si>
+    <t>St. Lawrence</t>
+  </si>
+  <si>
+    <t>principal@stlawrencehighschool.edu.in</t>
+  </si>
+  <si>
+    <t>03324751959/2539</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lakshmipathi Singhnia </t>
+  </si>
+  <si>
+    <t>Isa_kol@rediffmail.com</t>
+  </si>
+  <si>
+    <t>Army Public School</t>
+  </si>
+  <si>
+    <t>apskolkata94@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frank Anthony Public </t>
+  </si>
+  <si>
+    <t>fapscal@gmail.com</t>
+  </si>
+  <si>
+    <t>Gems Akademia</t>
+  </si>
+  <si>
+    <t>info@gemsakademia.in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vivekananda Mission </t>
+  </si>
+  <si>
+    <t>admin@vms.edu.in</t>
+  </si>
+  <si>
+    <t>K.E Carmel Sarisha</t>
+  </si>
+  <si>
+    <t>kecarmelsarisha@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP Ghosh Memorial  </t>
+  </si>
+  <si>
+    <t>info.baruipur@hpgmemorial.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St.Joseph Bright </t>
+  </si>
+  <si>
+    <t>sjbschool.amtala@gmail.com</t>
+  </si>
+  <si>
+    <t>SouthCity International</t>
+  </si>
+  <si>
+    <t>info@scis.co.in</t>
+  </si>
+  <si>
+    <t>PB Academy</t>
+  </si>
+  <si>
+    <t>pbacademischool@gmail.com</t>
+  </si>
+  <si>
+    <t>Mahavir Institute</t>
+  </si>
+  <si>
+    <t>United Missionary</t>
+  </si>
+  <si>
+    <t>umptti@gmail.com</t>
+  </si>
+  <si>
+    <t>St. Xaviers Public</t>
+  </si>
+  <si>
+    <t>The Summit</t>
+  </si>
+  <si>
+    <t>St. Clare</t>
+  </si>
+  <si>
+    <t>info@stclareschoolkolkata</t>
+  </si>
+  <si>
+    <t>Apeejay</t>
+  </si>
+  <si>
+    <t>principal.parkstreet@apeejayschool.com</t>
+  </si>
+  <si>
+    <t>Apeejay (Salt Lake)</t>
+  </si>
+  <si>
+    <t>principal.saltlake@apeejayschool.com</t>
+  </si>
+  <si>
+    <t>Hariyana Vidya Mandir</t>
+  </si>
+  <si>
+    <t>vidya@hariyanavidyamandir.org</t>
+  </si>
+  <si>
+    <t>Garden High (Sonarpur)</t>
+  </si>
+  <si>
+    <t>9830847607/9830337697</t>
+  </si>
+  <si>
+    <t>Saini International</t>
+  </si>
+  <si>
+    <t>09903683222/8094001822</t>
+  </si>
+  <si>
+    <t>Nalanda Vidyapeeth</t>
+  </si>
+  <si>
+    <t>Narayana (Barasat)</t>
+  </si>
+  <si>
+    <t>WBBARASAT.ETECHNO@NARAYANAGROUP.COM</t>
+  </si>
+  <si>
+    <t>Shri Santoshi Maa Academy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akshar School </t>
+  </si>
+  <si>
+    <t>God Shepherd</t>
+  </si>
+  <si>
+    <t>tgms@rediffmail.com</t>
+  </si>
+  <si>
+    <t>St Francis Elite</t>
+  </si>
+  <si>
+    <t>info@sfeschool.in</t>
+  </si>
+  <si>
+    <t>Oxford Academy</t>
+  </si>
+  <si>
+    <t>Bihani Academy</t>
+  </si>
+  <si>
+    <t>info@bihaniacademy.com</t>
+  </si>
+  <si>
+    <t>Alps Convent</t>
+  </si>
+  <si>
+    <t>Shree Bharati Academy</t>
+  </si>
+  <si>
+    <t>Sri Chaitanyo Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aditya Academy </t>
+  </si>
+  <si>
+    <t>Pearl Rosary High School</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,12 +502,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF653A2D"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -323,7 +524,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -343,7 +544,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -626,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1022,7 +1222,7 @@
       <c r="C22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="9" t="s">
         <v>54</v>
       </c>
       <c r="E22" s="1">
@@ -1073,25 +1273,527 @@
       <c r="C25" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="9"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D26" s="10"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D27" s="10"/>
+      <c r="D25" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="1">
+        <v>3324793241</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="1">
+        <v>3324344455</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B27" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="1">
+        <v>3340083093</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D28" s="10"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D31" s="6"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D32" s="6"/>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D33" s="6"/>
+      <c r="B28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="1">
+        <v>3324618002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B29" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" s="1">
+        <v>3324569090</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B31" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" s="1">
+        <v>3322233062</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B32" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B33" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E33" s="1">
+        <v>3324793600</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" s="1">
+        <v>3324866629</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B35" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E35" s="1">
+        <v>3322848038</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B36" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E36" s="1">
+        <v>905188888</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B37" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E37" s="1">
+        <v>7596949952</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B38" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E38" s="1">
+        <v>7478196910</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B39" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E39" s="1">
+        <v>7044447761</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B40" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E40" s="1">
+        <v>7059600647</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B41" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E41" s="1">
+        <v>3340072444</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B42" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E42" s="1">
+        <v>9903102957</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B43" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="1">
+        <v>7605080650</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B44" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E44" s="1">
+        <v>3324752135</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B45" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E45" s="1">
+        <v>9674645471</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B46" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E46" s="1">
+        <v>9073681886</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B47" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E47" s="1">
+        <v>3324316997</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B48" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E48" s="1">
+        <v>3322291779</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B49" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E49" s="1">
+        <v>3323215151</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B50" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E50" s="1">
+        <v>3323342404</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B51" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B52" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B53" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53" s="1">
+        <v>9606279184</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B54" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E54" s="1">
+        <v>8777867589</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B55" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E55" s="1">
+        <v>8017672075</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B56" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E56" s="1">
+        <v>3324492810</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B57" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E57" s="1">
+        <v>3324967196</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B58" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E58" s="1">
+        <v>9830701347</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B59" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E59" s="1">
+        <v>3324961723</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B60" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E60" s="1">
+        <v>9007792852</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B61" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E61" s="1">
+        <v>8902765583</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B62" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E62" s="1">
+        <v>9331866252</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B63" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E63" s="1">
+        <v>9903540099</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B64" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E64" s="1">
+        <v>8336998663</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B65" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E65" s="1">
+        <v>9339527506</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1109,9 +1811,36 @@
     <hyperlink ref="D22" r:id="rId12" xr:uid="{07F0AFEA-F8BD-4093-81BD-41EC84D474F1}"/>
     <hyperlink ref="D23" r:id="rId13" xr:uid="{C476D3FD-7619-4152-BF8B-DA12B03063BD}"/>
     <hyperlink ref="D24" r:id="rId14" xr:uid="{380E3A26-AE6E-419B-A807-E6BB4359E95A}"/>
+    <hyperlink ref="D25" r:id="rId15" xr:uid="{8C0E8A57-592C-459F-9CA4-EBAFF29B1461}"/>
+    <hyperlink ref="D26" r:id="rId16" xr:uid="{D8E12D83-7475-4118-9975-306187FD1E70}"/>
+    <hyperlink ref="D27" r:id="rId17" xr:uid="{1F12C2E0-6CC2-4D63-A436-8B947270B432}"/>
+    <hyperlink ref="D28" r:id="rId18" xr:uid="{D6CDABD5-1ADA-4959-B8CA-C26F7C9BDE9D}"/>
+    <hyperlink ref="D29" r:id="rId19" xr:uid="{FE8B5668-124A-4184-82D7-3536AE1CC8C7}"/>
+    <hyperlink ref="D30" r:id="rId20" xr:uid="{5B2DB390-F5A8-4F5C-A5F9-92CFC5BE4F20}"/>
+    <hyperlink ref="D31" r:id="rId21" xr:uid="{E4CF2DC6-980A-4A27-A256-BF716D9EA0C1}"/>
+    <hyperlink ref="D32" r:id="rId22" xr:uid="{2A0E41EB-3C24-490A-81CD-3CD747C54ED3}"/>
+    <hyperlink ref="D33" r:id="rId23" xr:uid="{929AACDF-9F87-4410-B171-A3B08294CFD5}"/>
+    <hyperlink ref="D34" r:id="rId24" xr:uid="{5CA76DF3-5342-410E-9F66-4EEC91703785}"/>
+    <hyperlink ref="D35" r:id="rId25" xr:uid="{8CE0FA44-ADD1-44A6-8844-E4B5368414A2}"/>
+    <hyperlink ref="D36" r:id="rId26" xr:uid="{86292120-F09F-42BC-BA9B-51309AB7E996}"/>
+    <hyperlink ref="D37" r:id="rId27" xr:uid="{F981F006-B922-4416-9524-8BE65F81BC24}"/>
+    <hyperlink ref="D38" r:id="rId28" xr:uid="{E1B2DDA0-73A3-4069-9ED0-3454AACCC089}"/>
+    <hyperlink ref="D39" r:id="rId29" xr:uid="{CB861D5A-C6E8-45A2-9941-AC035ADF70E2}"/>
+    <hyperlink ref="D40" r:id="rId30" xr:uid="{F94E5239-6337-4E4C-8F4F-1B4FBBEB0038}"/>
+    <hyperlink ref="D41" r:id="rId31" xr:uid="{1EA4A656-668B-419F-91D0-38B6DC87D752}"/>
+    <hyperlink ref="D42" r:id="rId32" xr:uid="{1A452B96-61F1-4524-8DFB-726C0C418FEC}"/>
+    <hyperlink ref="D44" r:id="rId33" xr:uid="{83C3A00E-6C64-4090-8CA7-20B6C0D8ADC8}"/>
+    <hyperlink ref="D47" r:id="rId34" xr:uid="{0647F456-BEFC-4615-AAF1-8FE12495C6BA}"/>
+    <hyperlink ref="D48" r:id="rId35" xr:uid="{29BC6F6C-32B9-4515-A979-3C1615422DA8}"/>
+    <hyperlink ref="D49" r:id="rId36" xr:uid="{0ECEA590-B7D9-403D-BF22-1D93436E6526}"/>
+    <hyperlink ref="D50" r:id="rId37" xr:uid="{9ECAF91A-36F4-4C19-9C1B-07932BBDC8F8}"/>
+    <hyperlink ref="D54" r:id="rId38" xr:uid="{8C1A0011-B460-4073-B9C6-CBF56F86FC5E}"/>
+    <hyperlink ref="D57" r:id="rId39" xr:uid="{D1EEB7D6-4B45-4D3D-9B6F-72685A51C52B}"/>
+    <hyperlink ref="D58" r:id="rId40" xr:uid="{19B65A80-0871-429A-A7E9-BA039EBEFD50}"/>
+    <hyperlink ref="D60" r:id="rId41" xr:uid="{D97F7317-7544-4822-82D0-4B861C0C24FB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
-  <legacyDrawing r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId42"/>
+  <legacyDrawing r:id="rId43"/>
 </worksheet>
 </file>
</xml_diff>